<commit_message>
todolist et petit icon
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\BNGRC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{705DA97D-B6AF-4806-87A6-9973BED2BFFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9763F48-B34E-463B-869F-4588EEC6211D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{A710062A-1674-48F6-A594-BBEDF4D07A77}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="46">
   <si>
     <t>Module</t>
   </si>
@@ -136,6 +136,45 @@
   </si>
   <si>
     <t>Liste des dons</t>
+  </si>
+  <si>
+    <t>base.sql</t>
+  </si>
+  <si>
+    <t>data.sql</t>
+  </si>
+  <si>
+    <t>vue.sql</t>
+  </si>
+  <si>
+    <t>Vue pour les fonctions</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>Version 1</t>
+  </si>
+  <si>
+    <t>Version 2</t>
+  </si>
+  <si>
+    <t>listeBesoinVille.php</t>
+  </si>
+  <si>
+    <t>Achat des besoins si il y a l'argent</t>
+  </si>
+  <si>
+    <t>simulation.php</t>
+  </si>
+  <si>
+    <t>Page de simulation des achats des validations</t>
+  </si>
+  <si>
+    <t>recapitulation.php</t>
+  </si>
+  <si>
+    <t>Page de recapitulation des besoins</t>
   </si>
 </sst>
 </file>
@@ -151,7 +190,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -161,6 +200,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -177,11 +222,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -496,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3202EAC-5BD7-4C25-9FFF-FEDE4B2E1BB8}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,40 +585,20 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2">
-        <v>10</v>
-      </c>
-      <c r="F2">
-        <v>10</v>
-      </c>
-      <c r="G2">
-        <f>E2-F2</f>
-        <v>0</v>
-      </c>
-      <c r="H2" s="2">
-        <f>F2/(F2+G2)%</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E3">
         <v>10</v>
@@ -581,35 +607,36 @@
         <v>10</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G7" si="0">E3-F3</f>
+        <f>E3-F3</f>
         <v>0</v>
       </c>
       <c r="H3" s="2">
-        <f t="shared" ref="H3:H8" si="1">F3/(F3+G3)%</f>
+        <f>F3/(F3+G3)%</f>
         <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E4">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F4">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="G4">
+        <f t="shared" ref="G4:G9" si="0">E4-F4</f>
         <v>0</v>
       </c>
       <c r="H4" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="H4:H10" si="1">F4/(F4+G4)%</f>
         <v>100</v>
       </c>
     </row>
@@ -617,17 +644,20 @@
       <c r="A5" t="s">
         <v>14</v>
       </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
         <v>15</v>
       </c>
       <c r="E5">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="F5">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -639,22 +669,22 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
         <v>15</v>
       </c>
       <c r="E6">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="F6">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -666,50 +696,46 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7">
-        <v>10</v>
-      </c>
-      <c r="F7">
-        <v>10</v>
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" t="s">
+        <v>37</v>
       </c>
       <c r="G7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H7" s="2">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
         <v>15</v>
       </c>
       <c r="E8">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F8">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -721,55 +747,56 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E9">
-        <v>30</v>
-      </c>
-      <c r="F9" s="3">
-        <v>30</v>
-      </c>
-      <c r="G9" s="3">
+        <v>10</v>
+      </c>
+      <c r="F9">
+        <v>10</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H9" s="2">
-        <f>F9/(F9+G9)%</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E10">
-        <v>10</v>
-      </c>
-      <c r="F10" s="3">
-        <v>10</v>
-      </c>
-      <c r="G10" s="3">
+        <v>25</v>
+      </c>
+      <c r="F10">
+        <v>20</v>
+      </c>
+      <c r="G10">
         <v>0</v>
       </c>
       <c r="H10" s="2">
-        <f>F10/(F10+G10)%</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
@@ -778,53 +805,222 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
         <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E11">
         <v>30</v>
       </c>
       <c r="F11" s="3">
-        <v>55</v>
-      </c>
-      <c r="G11">
+        <v>35</v>
+      </c>
+      <c r="G11" s="3">
         <v>0</v>
       </c>
       <c r="H11" s="2">
-        <f t="shared" ref="H11:H12" si="2">F11/(F11+G11)%</f>
-        <v>99.999999999999986</v>
+        <f>F11/(F11+G11)%</f>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12">
+        <v>10</v>
+      </c>
+      <c r="F12" s="3">
+        <v>10</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0</v>
+      </c>
+      <c r="H12" s="2">
+        <f>F12/(F12+G12)%</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13">
+        <v>30</v>
+      </c>
+      <c r="F13" s="3">
+        <v>55</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" ref="H13:H20" si="2">F13/(F13+G13)%</f>
+        <v>99.999999999999986</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>29</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B14" t="s">
         <v>30</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C14" t="s">
         <v>31</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D14" t="s">
         <v>13</v>
       </c>
-      <c r="E12">
-        <v>10</v>
-      </c>
-      <c r="F12" s="3">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>10</v>
-      </c>
-      <c r="H12" s="2">
+      <c r="E14">
+        <v>10</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>10</v>
+      </c>
+      <c r="H14" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17">
+        <v>10</v>
+      </c>
+      <c r="F17">
+        <v>10</v>
+      </c>
+      <c r="G17">
+        <f>E17-F17</f>
+        <v>0</v>
+      </c>
+      <c r="H17" s="2">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18">
+        <v>60</v>
+      </c>
+      <c r="F18">
+        <v>150</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19">
+        <v>60</v>
+      </c>
+      <c r="F19">
+        <v>180</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19" s="2">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20">
+        <v>120</v>
+      </c>
+      <c r="F20">
+        <v>90</v>
+      </c>
+      <c r="G20">
+        <v>60</v>
+      </c>
+      <c r="H20" s="2">
+        <f t="shared" si="2"/>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>